<commit_message>
Update 'text and logos'
</commit_message>
<xml_diff>
--- a/layers.xlsx
+++ b/layers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul.chiorean/Documents/GitHub/Indentz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379F4B40-0E72-2045-8EF1-50E1717EEEFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170E5E55-C4A9-9140-A7BB-E8CCD2E76269}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30280" yWindow="17560" windowWidth="30260" windowHeight="25640" xr2:uid="{42E9474B-5D3B-B94E-8B33-AD4B54FF1CC6}"/>
   </bookViews>
@@ -234,9 +234,6 @@
     <t>hw logo, logo hw, wh, whw</t>
   </si>
   <si>
-    <t>copy, text, textes, txt, type</t>
-  </si>
-  <si>
     <t>product, tins</t>
   </si>
   <si>
@@ -259,6 +256,9 @@
   </si>
   <si>
     <t>grid</t>
+  </si>
+  <si>
+    <t>copy, text, textes, txt, type, typo</t>
   </si>
 </sst>
 </file>
@@ -710,7 +710,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -779,7 +779,7 @@
         <v>21</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -837,7 +837,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -915,12 +915,12 @@
         <v>21</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>55</v>
@@ -935,7 +935,7 @@
         <v>21</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -955,7 +955,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -975,7 +975,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -995,7 +995,7 @@
         <v>20</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1015,7 +1015,7 @@
         <v>20</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Change TRUE/FALSE to yes/no
</commit_message>
<xml_diff>
--- a/layers.xlsx
+++ b/layers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul.chiorean/Documents/GitHub/Indentz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C34E98-035E-A04E-A1E3-3A540C381B8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200F8C0E-4380-B541-A818-137FF70DE89C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30280" yWindow="17560" windowWidth="30260" windowHeight="25640" xr2:uid="{42E9474B-5D3B-B94E-8B33-AD4B54FF1CC6}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="76">
   <si>
     <t>safe area</t>
   </si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>codes</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -710,7 +716,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -749,11 +755,11 @@
       <c r="B2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="b">
-        <v>1</v>
+      <c r="C2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>21</v>
@@ -769,11 +775,11 @@
       <c r="B3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5" t="b">
-        <v>1</v>
+      <c r="C3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>21</v>
@@ -789,11 +795,11 @@
       <c r="B4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5" t="b">
-        <v>1</v>
+      <c r="C4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>21</v>
@@ -809,11 +815,11 @@
       <c r="B5" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5" t="b">
-        <v>1</v>
+      <c r="C5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>21</v>
@@ -827,11 +833,11 @@
       <c r="B6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5" t="b">
-        <v>0</v>
+      <c r="C6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>21</v>
@@ -847,11 +853,11 @@
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5" t="b">
-        <v>1</v>
+      <c r="C7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>21</v>
@@ -867,11 +873,11 @@
       <c r="B8" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5" t="b">
-        <v>1</v>
+      <c r="C8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>21</v>
@@ -887,11 +893,11 @@
       <c r="B9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="5" t="b">
-        <v>1</v>
+      <c r="C9" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>21</v>
@@ -905,11 +911,11 @@
       <c r="B10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="5" t="b">
-        <v>1</v>
+      <c r="C10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>21</v>
@@ -925,11 +931,11 @@
       <c r="B11" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5" t="b">
-        <v>1</v>
+      <c r="C11" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>21</v>
@@ -945,11 +951,11 @@
       <c r="B12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="5" t="b">
-        <v>1</v>
+      <c r="C12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>21</v>
@@ -965,11 +971,11 @@
       <c r="B13" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="5" t="b">
-        <v>1</v>
+      <c r="C13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>21</v>
@@ -985,11 +991,11 @@
       <c r="B14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="5" t="b">
-        <v>1</v>
+      <c r="C14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>20</v>
@@ -1005,11 +1011,11 @@
       <c r="B15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="5" t="b">
-        <v>0</v>
+      <c r="C15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>20</v>
@@ -1135,7 +1141,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AECEF0-A6A2-E048-BFD7-E7F541FF3FF7}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1162,8 +1170,8 @@
       <c r="B2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="12" t="b">
-        <v>1</v>
+      <c r="C2" s="12" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1173,8 +1181,8 @@
       <c r="B3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="12" t="b">
-        <v>0</v>
+      <c r="C3" s="12" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Change TOP/BOTTOM to above/below
</commit_message>
<xml_diff>
--- a/layers.xlsx
+++ b/layers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul.chiorean/Documents/GitHub/Indentz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200F8C0E-4380-B541-A818-137FF70DE89C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C17E19A-39DA-D04C-8590-0A5F1623A283}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30280" yWindow="17560" windowWidth="30260" windowHeight="25640" xr2:uid="{42E9474B-5D3B-B94E-8B33-AD4B54FF1CC6}"/>
   </bookViews>
@@ -99,12 +99,6 @@
     <t>Order</t>
   </si>
   <si>
-    <t>bottom</t>
-  </si>
-  <si>
-    <t>top</t>
-  </si>
-  <si>
     <t>order</t>
   </si>
   <si>
@@ -265,6 +259,12 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>above</t>
+  </si>
+  <si>
+    <t>below</t>
   </si>
 </sst>
 </file>
@@ -753,19 +753,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -773,19 +773,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F3" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -793,19 +793,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F4" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -813,16 +813,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="F5" s="6"/>
     </row>
@@ -831,19 +831,19 @@
         <v>6</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F6" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -851,19 +851,19 @@
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F7" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -871,19 +871,19 @@
         <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F8" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -891,16 +891,16 @@
         <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="F9" s="6"/>
     </row>
@@ -909,39 +909,39 @@
         <v>10</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F10" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="D11" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F11" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -949,19 +949,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F12" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -969,19 +969,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F13" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -989,19 +989,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="F14" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1009,19 +1009,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="F15" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1142,7 +1142,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -1154,200 +1154,200 @@
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1357,7 +1357,7 @@
     </row>
     <row r="38" spans="1:1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sync to docs sample
</commit_message>
<xml_diff>
--- a/layers.xlsx
+++ b/layers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul.chiorean/Documents/GitHub/Indentz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4E8EABA-E8FD-714B-9463-063F217ED8A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1501F484-13F5-0947-94B1-3560F25446FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30280" yWindow="17560" windowWidth="30260" windowHeight="25640" xr2:uid="{42E9474B-5D3B-B94E-8B33-AD4B54FF1CC6}"/>
   </bookViews>
@@ -195,7 +195,7 @@
     <t>below</t>
   </si>
   <si>
-    <t>cut, cut lines, decoupe, die, die cut, stanze</t>
+    <t>cut*, decoupe, die, die*cut, stanz*</t>
   </si>
 </sst>
 </file>

</xml_diff>